<commit_message>
Update example filelist.xlsx contents
</commit_message>
<xml_diff>
--- a/data/filelist.xlsx
+++ b/data/filelist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CCD\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zvanderbosch\github\nightskies_fork\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B15CFB7-33BE-4DF0-AA49-9CC87DED9AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE765F27-0FDF-472B-8127-A19875190473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43470" yWindow="915" windowWidth="15420" windowHeight="6210" xr2:uid="{71AEDB74-11ED-472F-808D-DF4FD53F2C10}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20460" windowHeight="20115" xr2:uid="{71AEDB74-11ED-472F-808D-DF4FD53F2C10}"/>
   </bookViews>
   <sheets>
     <sheet name="filelist" sheetId="1" r:id="rId1"/>
@@ -83,25 +83,25 @@
     <t>NIOB240830</t>
   </si>
   <si>
-    <t>ZABA250503</t>
-  </si>
-  <si>
     <t>Process</t>
   </si>
   <si>
-    <t>Z Vanderbosch</t>
-  </si>
-  <si>
-    <t>Rocky Mountain_NP</t>
-  </si>
-  <si>
     <t>Niobrara NSR</t>
   </si>
   <si>
-    <t>Zachs Backyard</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>J Doe</t>
+  </si>
+  <si>
+    <t>Rocky Mountain NP</t>
+  </si>
+  <si>
+    <t>Grand Canyon NP</t>
+  </si>
+  <si>
+    <t>GRCA120730</t>
   </si>
 </sst>
 </file>
@@ -990,7 +990,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1010,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1066,13 +1066,13 @@
         <v>14.78</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="2">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1080,13 +1080,13 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -1101,21 +1101,21 @@
         <v>14.78</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" s="2">
         <v>180</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -1136,7 +1136,7 @@
         <v>14.78</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" s="2">
         <v>30</v>

</xml_diff>